<commit_message>
pushing before making huge changes
</commit_message>
<xml_diff>
--- a/presentation/results.xlsx
+++ b/presentation/results.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\SAR\presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497BFEF4-2885-4DBF-BDCC-C7073AAF16A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A340598-059D-417B-83D1-9A38F92D168B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="NormalPrefix" sheetId="1" r:id="rId1"/>
+    <sheet name="NormalPrefix+Star" sheetId="2" r:id="rId2"/>
+    <sheet name="NormalPrefix+1D" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,18 +35,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
   <si>
     <t>Prefix length</t>
   </si>
   <si>
-    <t>Total time (ns)</t>
-  </si>
-  <si>
     <t>Average time (ns)</t>
-  </si>
-  <si>
-    <t>Number of packets</t>
   </si>
   <si>
     <t>Median Total Time (ns)</t>
@@ -126,6 +122,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Average time (ns)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1050">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -166,7 +192,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>NormalPrefix!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -201,7 +227,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$33</c:f>
+              <c:f>NormalPrefix!$A$2:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -306,7 +332,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$33</c:f>
+              <c:f>NormalPrefix!$B$2:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -468,9 +494,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
                   <a:t>Prefix length</a:t>
                 </a:r>
+                <a:endParaRPr lang="en-US" sz="700">
+                  <a:effectLst/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -585,14 +616,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Average time</a:t>
+                  <a:rPr lang="en-US" sz="1200" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Average time per each packet</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> per each packet</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-US" sz="700">
+                  <a:effectLst/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -718,7 +749,1211 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Average time (ns)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1050">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'NormalPrefix+Star'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average time (ns)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'NormalPrefix+Star'!$A$2:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'NormalPrefix+Star'!$B$2:$B$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>114215</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>125311</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>126136</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>146343</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>124114</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>127098</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>161787</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>142792</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>130265</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>133892</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>131365</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>130480</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>123051</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>125918</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>135483</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>131596</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>128299</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>125978</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>148530</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>131114</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>131415</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>144318</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>143032</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>147265</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>144420</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>146276</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>139469</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>136091</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>139935</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>133868</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>149180</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>137039</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CB72-463C-8495-BFA1C3982A34}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1467024272"/>
+        <c:axId val="1524584208"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1467024272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Prefix length</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="700">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1524584208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1524584208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Average time per each packet</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="700">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1467024272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'NormalPrefix+1D'!$A$2:$A$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'NormalPrefix+1D'!$B$2:$B$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>4602</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6437</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4089</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5186</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4580</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5801</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4785</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4562</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4575</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4266</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3703</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5747</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3765</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5375</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4662</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4540</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4286</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4507</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4138</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5566</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4138</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8040</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>14142</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>27106</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>47892</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>78718</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>107524</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>129560</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>136481</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>134102</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>132668</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>140760</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FA36-4834-88C9-C65B250487F3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1406899727"/>
+        <c:axId val="1116620255"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1406899727"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1116620255"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1116620255"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1406899727"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1274,20 +2509,1052 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1457324</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1295,6 +3562,134 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C85DFC4C-8E9B-4FEC-A9A8-908C5DA87A28}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9523</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E83B4642-A224-49B0-9801-0C568953EF68}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.08146</cdr:x>
+      <cdr:y>0.94619</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.18111</cdr:x>
+      <cdr:y>0.99283</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42EB240C-3722-4FEF-8712-C02C32CBE9E5}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="895351" y="5024438"/>
+          <a:ext cx="1095375" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Added * rules</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96019163-0587-4879-BF63-E769F54D8F2A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1578,22 +3973,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
-    <col min="5" max="6" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1603,502 +3996,265 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>802892400</v>
+        <v>8029</v>
       </c>
       <c r="C2">
-        <f>ROUND(B2/D2,0)</f>
-        <v>8029</v>
-      </c>
-      <c r="D2">
-        <v>100000</v>
-      </c>
-      <c r="E2">
         <f>MEDIAN(B2:B33)</f>
-        <v>467787150</v>
-      </c>
-      <c r="F2">
-        <f>MEDIAN(C2:C33)</f>
         <v>4678</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>543824000</v>
-      </c>
-      <c r="C3">
-        <f>ROUND(B3/D3,0)</f>
         <v>5438</v>
       </c>
-      <c r="D3">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>470203500</v>
-      </c>
-      <c r="C4">
-        <f t="shared" ref="C4:C33" si="0">ROUND(B4/D4,0)</f>
         <v>4702</v>
       </c>
-      <c r="D4">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>459754100</v>
-      </c>
-      <c r="C5">
-        <f t="shared" si="0"/>
         <v>4598</v>
       </c>
-      <c r="D5">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>452896200</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
         <v>4529</v>
       </c>
-      <c r="D6">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>431227900</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
         <v>4312</v>
       </c>
-      <c r="D7">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>545638700</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
         <v>5456</v>
       </c>
-      <c r="D8">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>491058500</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
         <v>4911</v>
       </c>
-      <c r="D9">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>450979800</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="0"/>
         <v>4510</v>
       </c>
-      <c r="D10">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>630365400</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="0"/>
         <v>6304</v>
       </c>
-      <c r="D11">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>504981300</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="0"/>
         <v>5050</v>
       </c>
-      <c r="D12">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>457684900</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="0"/>
         <v>4577</v>
       </c>
-      <c r="D13">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>584294000</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="0"/>
         <v>5843</v>
       </c>
-      <c r="D14">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>448075200</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="0"/>
         <v>4481</v>
       </c>
-      <c r="D15">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>433413200</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="0"/>
         <v>4334</v>
       </c>
-      <c r="D16">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>448937300</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="0"/>
         <v>4489</v>
       </c>
-      <c r="D17">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>666863900</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="0"/>
         <v>6669</v>
       </c>
-      <c r="D18">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>465370800</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="0"/>
         <v>4654</v>
       </c>
-      <c r="D19">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>455508600</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="0"/>
         <v>4555</v>
       </c>
-      <c r="D20">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>485649100</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="0"/>
         <v>4856</v>
       </c>
-      <c r="D21">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
-        <v>470745200</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="0"/>
         <v>4707</v>
       </c>
-      <c r="D22">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
-        <v>442579500</v>
-      </c>
-      <c r="C23">
-        <f t="shared" si="0"/>
         <v>4426</v>
       </c>
-      <c r="D23">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>443374500</v>
-      </c>
-      <c r="C24">
-        <f t="shared" si="0"/>
         <v>4434</v>
       </c>
-      <c r="D24">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
-        <v>436630200</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="0"/>
         <v>4366</v>
       </c>
-      <c r="D25">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26">
-        <v>442623500</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="0"/>
         <v>4426</v>
       </c>
-      <c r="D26">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27">
-        <v>446674800</v>
-      </c>
-      <c r="C27">
-        <f t="shared" si="0"/>
         <v>4467</v>
       </c>
-      <c r="D27">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28">
-        <v>483837200</v>
-      </c>
-      <c r="C28">
-        <f t="shared" si="0"/>
         <v>4838</v>
       </c>
-      <c r="D28">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29">
-        <v>445173200</v>
-      </c>
-      <c r="C29">
-        <f t="shared" si="0"/>
         <v>4452</v>
       </c>
-      <c r="D29">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30">
-        <v>585435700</v>
-      </c>
-      <c r="C30">
-        <f t="shared" si="0"/>
         <v>5854</v>
       </c>
-      <c r="D30">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31">
-        <v>482932000</v>
-      </c>
-      <c r="C31">
-        <f t="shared" si="0"/>
         <v>4829</v>
       </c>
-      <c r="D31">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32">
-        <v>657457200</v>
-      </c>
-      <c r="C32">
-        <f t="shared" si="0"/>
         <v>6575</v>
       </c>
-      <c r="D32">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33">
-        <v>501145700</v>
-      </c>
-      <c r="C33">
-        <f t="shared" si="0"/>
         <v>5011</v>
-      </c>
-      <c r="D33">
-        <v>100000</v>
       </c>
     </row>
   </sheetData>
@@ -2106,4 +4262,591 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43AECE1B-5DB3-41ED-B38E-7DFB5B8797EF}">
+  <dimension ref="A1:C33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="A28:C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>114215</v>
+      </c>
+      <c r="C2">
+        <f>MEDIAN(B2:B33)</f>
+        <v>133880</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>125311</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>126136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>146343</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>124114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>127098</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>161787</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>142792</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>130265</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>133892</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>131365</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>130480</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>123051</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>125918</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>135483</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>131596</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>128299</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>125978</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>148530</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>131114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>131415</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>144318</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>143032</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>147265</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>144420</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>146276</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>139469</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>136091</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>139935</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>133868</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>149180</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>137039</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F09498DA-5388-4CEB-A9F6-7E69F828F738}">
+  <dimension ref="A1:C33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>32</v>
+      </c>
+      <c r="B2">
+        <v>4602</v>
+      </c>
+      <c r="C2">
+        <f>ROUND(MEDIAN(B2:B33),0)</f>
+        <v>5281</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>31</v>
+      </c>
+      <c r="B3">
+        <v>6437</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>4089</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>29</v>
+      </c>
+      <c r="B5">
+        <v>5186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>28</v>
+      </c>
+      <c r="B6">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>27</v>
+      </c>
+      <c r="B7">
+        <v>5801</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>26</v>
+      </c>
+      <c r="B8">
+        <v>4785</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>25</v>
+      </c>
+      <c r="B9">
+        <v>4562</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>4575</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <v>4266</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>22</v>
+      </c>
+      <c r="B12">
+        <v>3703</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>5747</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>3765</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>5375</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>4662</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>4540</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>4286</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>4507</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>14</v>
+      </c>
+      <c r="B20">
+        <v>4138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>13</v>
+      </c>
+      <c r="B21">
+        <v>5566</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>12</v>
+      </c>
+      <c r="B22">
+        <v>4138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>11</v>
+      </c>
+      <c r="B23">
+        <v>8040</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>10</v>
+      </c>
+      <c r="B24">
+        <v>14142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>27106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>8</v>
+      </c>
+      <c r="B26">
+        <v>47892</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>7</v>
+      </c>
+      <c r="B27">
+        <v>78718</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>6</v>
+      </c>
+      <c r="B28">
+        <v>107524</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>129560</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30">
+        <v>136481</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>3</v>
+      </c>
+      <c r="B31">
+        <v>134102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32">
+        <v>132668</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>140760</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C33">
+    <sortCondition descending="1" ref="A2"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>